<commit_message>
updated tris cal date in phProbe_SEEP file
</commit_message>
<xml_diff>
--- a/Data/August2021/CarbonateChemistry/phProbe_SEEP_2022_02_10.xlsx
+++ b/Data/August2021/CarbonateChemistry/phProbe_SEEP_2022_02_10.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/Documents/R_sessions/silbiger_lab/MooreaSGD_site-selection/Data/August2021/CarbonateChemistry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAA7874-6408-BB48-8B07-38CF6A17C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589ADFFE-958A-5A43-9796-138D98008D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="0" windowWidth="24620" windowHeight="14860" xr2:uid="{5A21872E-596D-8B4A-9981-CDB29B61F2B9}"/>
+    <workbookView xWindow="980" yWindow="0" windowWidth="24620" windowHeight="14860" xr2:uid="{5A21872E-596D-8B4A-9981-CDB29B61F2B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$33</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="48">
   <si>
     <t>CowTagID</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>TrisCalDate</t>
-  </si>
-  <si>
-    <t>No_Junk_Run</t>
   </si>
   <si>
     <t>Notes</t>
@@ -547,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89480924-2760-6040-AD9A-FAFE4679F420}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,7 +556,7 @@
     <col min="8" max="8" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,22 +587,19 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="1">
         <v>44412</v>
@@ -619,26 +613,25 @@
       <c r="H2" s="3">
         <v>-71.3</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I2" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1">
         <v>44412</v>
@@ -652,26 +645,25 @@
       <c r="H3" s="3">
         <v>-71.599999999999994</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I3" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1">
         <v>44413</v>
@@ -685,26 +677,25 @@
       <c r="H4" s="3">
         <v>-61.7</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I4" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1">
         <v>44413</v>
@@ -718,26 +709,25 @@
       <c r="H5" s="3">
         <v>-65.599999999999994</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1">
         <v>44413</v>
@@ -751,26 +741,25 @@
       <c r="H6" s="3">
         <v>-65.099999999999994</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
         <v>44413</v>
@@ -784,32 +773,31 @@
       <c r="H7" s="3">
         <v>-70</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>44413</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="4">
         <v>11.932</v>
@@ -817,32 +805,31 @@
       <c r="H8" s="3">
         <v>-75.599999999999994</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1">
         <v>44413</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="4">
         <v>5.9470000000000001</v>
@@ -850,26 +837,25 @@
       <c r="H9" s="3">
         <v>-71.5</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1">
         <v>44414</v>
@@ -883,26 +869,25 @@
       <c r="H10" s="3">
         <v>-71.3</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
         <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
       </c>
       <c r="E11" s="1">
         <v>44414</v>
@@ -916,26 +901,25 @@
       <c r="H11" s="3">
         <v>-62.5</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I11" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1">
         <v>44416</v>
@@ -949,26 +933,25 @@
       <c r="H12" s="3">
         <v>-74.3</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I12" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
       </c>
       <c r="E13" s="1">
         <v>44416</v>
@@ -982,26 +965,25 @@
       <c r="H13" s="3">
         <v>-66.2</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>44602</v>
+      </c>
       <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="1">
         <v>44417</v>
@@ -1015,26 +997,25 @@
       <c r="H14" s="3">
         <v>-63.9</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>44602</v>
+      </c>
       <c r="J14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="K14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1">
         <v>44416</v>
@@ -1048,26 +1029,25 @@
       <c r="H15" s="3">
         <v>-56.3</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="6">
         <v>44417</v>
@@ -1081,26 +1061,25 @@
       <c r="H16" s="9">
         <v>-56.1</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5" t="s">
+      <c r="I16" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="6">
         <v>44417</v>
@@ -1114,26 +1093,25 @@
       <c r="H17" s="9">
         <v>-64.8</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5" t="s">
+      <c r="I17" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1">
         <v>44417</v>
@@ -1147,26 +1125,25 @@
       <c r="H18" s="3">
         <v>-63.1</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I18" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1">
         <v>44417</v>
@@ -1180,26 +1157,25 @@
       <c r="H19" s="3">
         <v>-61.6</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I19" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1">
         <v>44417</v>
@@ -1213,26 +1189,25 @@
       <c r="H20" s="3">
         <v>-53</v>
       </c>
-      <c r="I20" s="1"/>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I20" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1">
         <v>44417</v>
@@ -1246,26 +1221,25 @@
       <c r="H21" s="3">
         <v>-60.7</v>
       </c>
-      <c r="I21" s="1"/>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I21" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1">
         <v>44417</v>
@@ -1279,26 +1253,25 @@
       <c r="H22" s="3">
         <v>-66.7</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I22" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1">
         <v>44417</v>
@@ -1312,26 +1285,25 @@
       <c r="H23" s="3">
         <v>-61.4</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I23" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
         <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>14</v>
       </c>
       <c r="E24" s="1">
         <v>44417</v>
@@ -1345,26 +1317,25 @@
       <c r="H24" s="3">
         <v>-64</v>
       </c>
-      <c r="I24" s="1"/>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I24" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1">
         <v>44417</v>
@@ -1378,26 +1349,25 @@
       <c r="H25" s="3">
         <v>-59.3</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I25" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1">
         <v>44418</v>
@@ -1411,26 +1381,25 @@
       <c r="H26" s="3">
         <v>-59</v>
       </c>
-      <c r="I26" s="1"/>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I26" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27" s="1">
         <v>44418</v>
@@ -1444,26 +1413,25 @@
       <c r="H27" s="3">
         <v>-59.1</v>
       </c>
-      <c r="I27" s="1"/>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I27" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E28" s="1">
         <v>44417</v>
@@ -1477,32 +1445,31 @@
       <c r="H28" s="3">
         <v>-56.5</v>
       </c>
-      <c r="I28" s="1"/>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="I28" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>44</v>
-      </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="1">
         <v>44358</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="4">
         <v>6.8550000000000004</v>
@@ -1510,32 +1477,31 @@
       <c r="H29" s="3">
         <v>-58.4</v>
       </c>
-      <c r="I29" s="1"/>
+      <c r="I29" s="1">
+        <v>44602</v>
+      </c>
       <c r="J29" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>46</v>
-      </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1">
         <v>44358</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G30" s="4">
         <v>7.1120000000000001</v>
@@ -1543,32 +1509,31 @@
       <c r="H30" s="3">
         <v>-57.6</v>
       </c>
-      <c r="I30" s="1"/>
+      <c r="I30" s="1">
+        <v>44602</v>
+      </c>
       <c r="J30" t="s">
-        <v>15</v>
-      </c>
-      <c r="K30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E31" s="1">
         <v>44417</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" s="4">
         <v>5.1020000000000003</v>
@@ -1576,26 +1541,25 @@
       <c r="H31" s="3">
         <v>-56.1</v>
       </c>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1">
+        <v>44602</v>
+      </c>
       <c r="J31" t="s">
-        <v>15</v>
-      </c>
-      <c r="K31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
         <v>13</v>
-      </c>
-      <c r="D32" t="s">
-        <v>14</v>
       </c>
       <c r="E32" s="1">
         <v>44416</v>
@@ -1609,26 +1573,25 @@
       <c r="H32" s="3">
         <v>-60.1</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I32" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1">
         <v>44418</v>
@@ -1642,12 +1605,11 @@
       <c r="H33" s="3">
         <v>-61.6</v>
       </c>
-      <c r="I33" s="1"/>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33" t="s">
-        <v>32</v>
+      <c r="I33" s="1">
+        <v>44602</v>
+      </c>
+      <c r="J33" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>